<commit_message>
change8 - after avneradania1 added change6 from zombie
</commit_message>
<xml_diff>
--- a/avner-excel.xlsx
+++ b/avner-excel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="248">
   <si>
     <t>Source-Dest type</t>
   </si>
@@ -595,181 +595,220 @@
     </r>
   </si>
   <si>
+    <t>Top die - C4 bump-7</t>
+  </si>
+  <si>
+    <t>i_next_top.i_periphery_top.i_periphery_top_i2c_io_wrap.i_jtag_tap_io_wrap.tap_tr_tck_iobuf.genblk1.i_gpio_tap</t>
+  </si>
+  <si>
+    <t>TEST__TR_TCK</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>L_TEST__TR_TCK</t>
+    </r>
+  </si>
+  <si>
+    <t>C4_TEST__TR_TCK</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>C4_TEST__TR_TCK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>TEST__TR_TCK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>=IF(F8="","",IF(A8="Top die - HBM","SII_L_"&amp;F8,"L_"&amp;F8))</t>
+    </r>
+  </si>
+  <si>
+    <t>C_TEST__TR_TCK</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>=IF(AN8="","","C_"&amp;RIGHT(AN8,LEN(AN8)−3))</t>
+    </r>
+  </si>
+  <si>
+    <t>Top die - C4 bump-8</t>
+  </si>
+  <si>
+    <t>i_next_top.i_periphery_top.i_periphery_top_i2c_io_wrap.i_jtag_tap_io_wrap.tap_pad_tri_l_iobuf.genblk1.i_gpio_tap</t>
+  </si>
+  <si>
+    <t>TEST__PAD_TRI_L</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>L_TEST__PAD_TRI_L</t>
+    </r>
+  </si>
+  <si>
+    <t>C4_TEST__PAD_TRI_L</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>C4_TEST__PAD_TRI_L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>TEST__PAD_TRI_L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>=IF(F9="","",IF(A9="Top die - HBM","SII_L_"&amp;F9,"L_"&amp;F9))</t>
+    </r>
+  </si>
+  <si>
+    <t>C_TEST__PAD_TRI_L</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>=IF(AN9="","","C_"&amp;RIGHT(AN9,LEN(AN9)−3))</t>
+    </r>
+  </si>
+  <si>
+    <t>Top die - C4 bump-9</t>
+  </si>
+  <si>
+    <t>I2C SBUS Master</t>
+  </si>
+  <si>
+    <t>E1825V_ODTRAN</t>
+  </si>
+  <si>
+    <t>periphery_top_i2c_io_wrap</t>
+  </si>
+  <si>
+    <t>i_next_top.i_periphery_top.i_periphery_top_i2c_io_wrap.i_twi_sbus_master_sda.genblk1.i_gpio_odtran</t>
+  </si>
+  <si>
+    <t>I2C_PERIPH_SBUS_M_SDA</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>0x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> i2c_periph_sbus_master</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>L_I2C_PERIPH_SBUS_M_SDA</t>
+    </r>
+  </si>
+  <si>
+    <t>C4_I2C_PERIPH_SBUS_M_SDA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>C4_I2C_PERIPH_SBUS_M_SDA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>I2C_PERIPH_SBUS_M_SDA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>=IF(F10="","",IF(A10="Top die - HBM","SII_L_"&amp;F10,"L_"&amp;F10))</t>
+    </r>
+  </si>
+  <si>
+    <t>C_I2C_PERIPH_SBUS_M_SDA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>=IF(AN10="","","C_"&amp;RIGHT(AN10,LEN(AN10)−3))</t>
+    </r>
+  </si>
+  <si>
     <t>Top die - C4 bump</t>
-  </si>
-  <si>
-    <t>i_next_top.i_periphery_top.i_periphery_top_i2c_io_wrap.i_jtag_tap_io_wrap.tap_tr_tck_iobuf.genblk1.i_gpio_tap</t>
-  </si>
-  <si>
-    <t>TEST__TR_TCK</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>L_TEST__TR_TCK</t>
-    </r>
-  </si>
-  <si>
-    <t>C4_TEST__TR_TCK</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>C4_TEST__TR_TCK</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>=IF(F8="","",IF(A8="Top die - HBM","SII_L_"&amp;F8,"L_"&amp;F8))</t>
-    </r>
-  </si>
-  <si>
-    <t>C_TEST__TR_TCK</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>=IF(AN8="","","C_"&amp;RIGHT(AN8,LEN(AN8)−3))</t>
-    </r>
-  </si>
-  <si>
-    <t>i_next_top.i_periphery_top.i_periphery_top_i2c_io_wrap.i_jtag_tap_io_wrap.tap_pad_tri_l_iobuf.genblk1.i_gpio_tap</t>
-  </si>
-  <si>
-    <t>TEST__PAD_TRI_L</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>L_TEST__PAD_TRI_L</t>
-    </r>
-  </si>
-  <si>
-    <t>C4_TEST__PAD_TRI_L</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>C4_TEST__PAD_TRI_L</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>=IF(F9="","",IF(A9="Top die - HBM","SII_L_"&amp;F9,"L_"&amp;F9))</t>
-    </r>
-  </si>
-  <si>
-    <t>C_TEST__PAD_TRI_L</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>=IF(AN9="","","C_"&amp;RIGHT(AN9,LEN(AN9)−3))</t>
-    </r>
-  </si>
-  <si>
-    <t>I2C SBUS Master</t>
-  </si>
-  <si>
-    <t>E1825V_ODTRAN</t>
-  </si>
-  <si>
-    <t>periphery_top_i2c_io_wrap</t>
-  </si>
-  <si>
-    <t>i_next_top.i_periphery_top.i_periphery_top_i2c_io_wrap.i_twi_sbus_master_sda.genblk1.i_gpio_odtran</t>
-  </si>
-  <si>
-    <t>I2C_PERIPH_SBUS_M_SDA</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>0x2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> i2c_periph_sbus_master</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>L_I2C_PERIPH_SBUS_M_SDA</t>
-    </r>
-  </si>
-  <si>
-    <t>C4_I2C_PERIPH_SBUS_M_SDA</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>C4_I2C_PERIPH_SBUS_M_SDA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>=IF(F10="","",IF(A10="Top die - HBM","SII_L_"&amp;F10,"L_"&amp;F10))</t>
-    </r>
-  </si>
-  <si>
-    <t>C_I2C_PERIPH_SBUS_M_SDA</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>=IF(AN10="","","C_"&amp;RIGHT(AN10,LEN(AN10)−3))</t>
-    </r>
   </si>
   <si>
     <t>i_next_top.i_periphery_top.i_periphery_top_i2c_io_wrap.i_twi_sbus_master_scl.genblk1.i_gpio_odtran</t>
@@ -3731,7 +3770,6 @@
       </c>
       <c r="AI8" t="s" s="14">
         <f>IF(LEFT(F8,3)="NC_","",IF(OR(A8="Top die - C4 bump",A8="Top die - HBM"),IF(G8="inout","inout",IF(G8="input","output",IF(G8="output","input"))),""))</f>
-        <v>63</v>
       </c>
       <c r="AJ8" s="15"/>
       <c r="AK8" t="s" s="16">
@@ -3742,7 +3780,6 @@
       </c>
       <c r="AM8" t="s" s="18">
         <f>IF(A8="Top die - C4 bump",IF(AI8="inout","inout",IF(AI8="input","output",IF(AI8="output","input",""))),IF(A8="HBM - C4 bump",IF(AK8="inout","inout",IF(AK8="input","output",IF(AK8="output","input"))),""))</f>
-        <v>63</v>
       </c>
       <c r="AN8" t="s" s="19">
         <f>AL8</f>
@@ -3750,15 +3787,13 @@
       </c>
       <c r="AO8" t="s" s="19">
         <f>IF(AM8="inout","inout",IF(AM8="input","output",IF(AM8="output","input","")))</f>
-        <v>63</v>
       </c>
       <c r="AP8" t="s" s="19">
         <f>IF(AR8="Point-To-Point","HBM_"&amp;AU8&amp;"_DA"&amp;AS8,IF(AR8="Multi-Drop","HBM_"&amp;AT8&amp;"_DA"&amp;AS8,IF(AR8="High-Z","",IF(AN8="","",RIGHT(AN8,LEN(AN8)-3)))))</f>
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="AQ8" t="s" s="19">
         <f>IF(AO8="inout","inout",IF(AO8="input","output",IF(AO8="output","input","")))</f>
-        <v>63</v>
       </c>
       <c r="AR8" s="20"/>
       <c r="AS8" s="19"/>
@@ -3781,7 +3816,7 @@
       </c>
       <c r="AZ8" t="s" s="8">
         <f>_xlfn.FORMULATEXT(AY8)</f>
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BA8" t="b" s="22">
         <f>EXACT(TRIM(_xlfn.FORMULATEXT(AP8)),TRIM(BC8))</f>
@@ -3789,18 +3824,18 @@
       </c>
       <c r="BB8" t="s" s="8">
         <f>IF(AN8="","","C_"&amp;RIGHT(AN8,LEN(AN8)-3))</f>
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="BC8" t="s" s="8">
         <f>_xlfn.FORMULATEXT(BB8)</f>
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="BD8" s="23"/>
       <c r="BE8" s="23"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" t="s" s="7">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s" s="8">
         <v>58</v>
@@ -3812,10 +3847,10 @@
         <v>60</v>
       </c>
       <c r="E9" t="s" s="8">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F9" t="s" s="9">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G9" t="s" s="10">
         <v>63</v>
@@ -3874,38 +3909,34 @@
       <c r="AG9" s="11"/>
       <c r="AH9" t="s" s="13">
         <f>IF(OR(F9="",LEFT(F9,3)="NC_"),"",IF(A9="Top die - HBM","SII_L_"&amp;F9,"L_"&amp;F9))</f>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AI9" t="s" s="14">
         <f>IF(LEFT(F9,3)="NC_","",IF(OR(A9="Top die - C4 bump",A9="Top die - HBM"),IF(G9="inout","inout",IF(G9="input","output",IF(G9="output","input"))),""))</f>
-        <v>63</v>
       </c>
       <c r="AJ9" s="15"/>
       <c r="AK9" t="s" s="16">
         <f>IF(A9="HBM - C4 bump","inout",IF(A9="Top die - HBM",IF(AI9="inout","inout",IF(AI9="input","output",IF(AI9="output","input"))),""))</f>
       </c>
       <c r="AL9" t="s" s="17">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AM9" t="s" s="18">
         <f>IF(A9="Top die - C4 bump",IF(AI9="inout","inout",IF(AI9="input","output",IF(AI9="output","input",""))),IF(A9="HBM - C4 bump",IF(AK9="inout","inout",IF(AK9="input","output",IF(AK9="output","input"))),""))</f>
-        <v>63</v>
       </c>
       <c r="AN9" t="s" s="19">
         <f>AL9</f>
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AO9" t="s" s="19">
         <f>IF(AM9="inout","inout",IF(AM9="input","output",IF(AM9="output","input","")))</f>
-        <v>63</v>
       </c>
       <c r="AP9" t="s" s="19">
         <f>IF(AR9="Point-To-Point","HBM_"&amp;AU9&amp;"_DA"&amp;AS9,IF(AR9="Multi-Drop","HBM_"&amp;AT9&amp;"_DA"&amp;AS9,IF(AR9="High-Z","",IF(AN9="","",RIGHT(AN9,LEN(AN9)-3)))))</f>
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="AQ9" t="s" s="19">
         <f>IF(AO9="inout","inout",IF(AO9="input","output",IF(AO9="output","input","")))</f>
-        <v>63</v>
       </c>
       <c r="AR9" s="20"/>
       <c r="AS9" s="19"/>
@@ -3924,11 +3955,11 @@
       </c>
       <c r="AY9" t="s" s="8">
         <f>IF(F9="","",IF(A9="Top die - HBM","SII_L_"&amp;F9,"L_"&amp;F9))</f>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AZ9" t="s" s="8">
         <f>_xlfn.FORMULATEXT(AY9)</f>
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="BA9" t="b" s="22">
         <f>EXACT(TRIM(_xlfn.FORMULATEXT(AP9)),TRIM(BC9))</f>
@@ -3936,33 +3967,33 @@
       </c>
       <c r="BB9" t="s" s="8">
         <f>IF(AN9="","","C_"&amp;RIGHT(AN9,LEN(AN9)-3))</f>
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="BC9" t="s" s="8">
         <f>_xlfn.FORMULATEXT(BB9)</f>
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="BD9" s="23"/>
       <c r="BE9" s="23"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s" s="8">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s" s="8">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D10" t="s" s="8">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s" s="8">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F10" t="s" s="9">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="G10" t="s" s="10">
         <v>63</v>
@@ -3991,10 +4022,10 @@
         <v>65</v>
       </c>
       <c r="S10" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="T10" t="s" s="10">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="U10" s="11"/>
       <c r="V10" t="s" s="10">
@@ -4021,42 +4052,38 @@
         <v>65</v>
       </c>
       <c r="AG10" t="s" s="10">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="AH10" t="s" s="13">
         <f>IF(OR(F10="",LEFT(F10,3)="NC_"),"",IF(A10="Top die - HBM","SII_L_"&amp;F10,"L_"&amp;F10))</f>
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="AI10" t="s" s="14">
         <f>IF(LEFT(F10,3)="NC_","",IF(OR(A10="Top die - C4 bump",A10="Top die - HBM"),IF(G10="inout","inout",IF(G10="input","output",IF(G10="output","input"))),""))</f>
-        <v>63</v>
       </c>
       <c r="AJ10" s="15"/>
       <c r="AK10" t="s" s="16">
         <f>IF(A10="HBM - C4 bump","inout",IF(A10="Top die - HBM",IF(AI10="inout","inout",IF(AI10="input","output",IF(AI10="output","input"))),""))</f>
       </c>
       <c r="AL10" t="s" s="17">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="AM10" t="s" s="18">
         <f>IF(A10="Top die - C4 bump",IF(AI10="inout","inout",IF(AI10="input","output",IF(AI10="output","input",""))),IF(A10="HBM - C4 bump",IF(AK10="inout","inout",IF(AK10="input","output",IF(AK10="output","input"))),""))</f>
-        <v>63</v>
       </c>
       <c r="AN10" t="s" s="19">
         <f>AL10</f>
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="AO10" t="s" s="19">
         <f>IF(AM10="inout","inout",IF(AM10="input","output",IF(AM10="output","input","")))</f>
-        <v>63</v>
       </c>
       <c r="AP10" t="s" s="19">
         <f>IF(AR10="Point-To-Point","HBM_"&amp;AU10&amp;"_DA"&amp;AS10,IF(AR10="Multi-Drop","HBM_"&amp;AT10&amp;"_DA"&amp;AS10,IF(AR10="High-Z","",IF(AN10="","",RIGHT(AN10,LEN(AN10)-3)))))</f>
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="AQ10" t="s" s="19">
         <f>IF(AO10="inout","inout",IF(AO10="input","output",IF(AO10="output","input","")))</f>
-        <v>63</v>
       </c>
       <c r="AR10" s="20"/>
       <c r="AS10" s="19"/>
@@ -4075,11 +4102,11 @@
       </c>
       <c r="AY10" t="s" s="8">
         <f>IF(F10="","",IF(A10="Top die - HBM","SII_L_"&amp;F10,"L_"&amp;F10))</f>
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="AZ10" t="s" s="8">
         <f>_xlfn.FORMULATEXT(AY10)</f>
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="BA10" t="b" s="22">
         <f>EXACT(TRIM(_xlfn.FORMULATEXT(AP10)),TRIM(BC10))</f>
@@ -4087,33 +4114,33 @@
       </c>
       <c r="BB10" t="s" s="8">
         <f>IF(AN10="","","C_"&amp;RIGHT(AN10,LEN(AN10)-3))</f>
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="BC10" t="s" s="8">
         <f>_xlfn.FORMULATEXT(BB10)</f>
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="BD10" s="23"/>
       <c r="BE10" s="23"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B11" t="s" s="8">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s" s="8">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D11" t="s" s="8">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s" s="8">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F11" t="s" s="9">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="G11" t="s" s="10">
         <v>63</v>
@@ -4142,10 +4169,10 @@
         <v>65</v>
       </c>
       <c r="S11" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="T11" t="s" s="10">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="U11" s="11"/>
       <c r="V11" t="s" s="10">
@@ -4172,11 +4199,11 @@
         <v>65</v>
       </c>
       <c r="AG11" t="s" s="10">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="AH11" t="s" s="13">
         <f>IF(OR(F11="",LEFT(F11,3)="NC_"),"",IF(A11="Top die - HBM","SII_L_"&amp;F11,"L_"&amp;F11))</f>
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="AI11" t="s" s="14">
         <f>IF(LEFT(F11,3)="NC_","",IF(OR(A11="Top die - C4 bump",A11="Top die - HBM"),IF(G11="inout","inout",IF(G11="input","output",IF(G11="output","input"))),""))</f>
@@ -4187,7 +4214,7 @@
         <f>IF(A11="HBM - C4 bump","inout",IF(A11="Top die - HBM",IF(AI11="inout","inout",IF(AI11="input","output",IF(AI11="output","input"))),""))</f>
       </c>
       <c r="AL11" t="s" s="17">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="AM11" t="s" s="18">
         <f>IF(A11="Top die - C4 bump",IF(AI11="inout","inout",IF(AI11="input","output",IF(AI11="output","input",""))),IF(A11="HBM - C4 bump",IF(AK11="inout","inout",IF(AK11="input","output",IF(AK11="output","input"))),""))</f>
@@ -4195,7 +4222,7 @@
       </c>
       <c r="AN11" t="s" s="19">
         <f>AL11</f>
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="AO11" t="s" s="19">
         <f>IF(AM11="inout","inout",IF(AM11="input","output",IF(AM11="output","input","")))</f>
@@ -4203,7 +4230,7 @@
       </c>
       <c r="AP11" t="s" s="19">
         <f>IF(AR11="Point-To-Point","HBM_"&amp;AU11&amp;"_DA"&amp;AS11,IF(AR11="Multi-Drop","HBM_"&amp;AT11&amp;"_DA"&amp;AS11,IF(AR11="High-Z","",IF(AN11="","",RIGHT(AN11,LEN(AN11)-3)))))</f>
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="AQ11" t="s" s="19">
         <f>IF(AO11="inout","inout",IF(AO11="input","output",IF(AO11="output","input","")))</f>
@@ -4226,11 +4253,11 @@
       </c>
       <c r="AY11" t="s" s="8">
         <f>IF(F11="","",IF(A11="Top die - HBM","SII_L_"&amp;F11,"L_"&amp;F11))</f>
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="AZ11" t="s" s="8">
         <f>_xlfn.FORMULATEXT(AY11)</f>
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="BA11" t="b" s="22">
         <f>EXACT(TRIM(_xlfn.FORMULATEXT(AP11)),TRIM(BC11))</f>
@@ -4238,36 +4265,36 @@
       </c>
       <c r="BB11" t="s" s="8">
         <f>IF(AN11="","","C_"&amp;RIGHT(AN11,LEN(AN11)-3))</f>
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="BC11" t="s" s="8">
         <f>_xlfn.FORMULATEXT(BB11)</f>
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="BD11" s="23"/>
       <c r="BE11" s="23"/>
     </row>
     <row r="12" ht="13.55" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B12" t="s" s="8">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C12" t="s" s="8">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D12" t="s" s="8">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="E12" t="s" s="8">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="F12" t="s" s="9">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="G12" t="s" s="10">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H12" t="s" s="10">
         <v>64</v>
@@ -4325,38 +4352,38 @@
       <c r="AG12" s="11"/>
       <c r="AH12" t="s" s="13">
         <f>IF(OR(F12="",LEFT(F12,3)="NC_"),"",IF(A12="Top die - HBM","SII_L_"&amp;F12,"L_"&amp;F12))</f>
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="AI12" t="s" s="14">
         <f>IF(LEFT(F12,3)="NC_","",IF(OR(A12="Top die - C4 bump",A12="Top die - HBM"),IF(G12="inout","inout",IF(G12="input","output",IF(G12="output","input"))),""))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AJ12" s="15"/>
       <c r="AK12" t="s" s="16">
         <f>IF(A12="HBM - C4 bump","inout",IF(A12="Top die - HBM",IF(AI12="inout","inout",IF(AI12="input","output",IF(AI12="output","input"))),""))</f>
       </c>
       <c r="AL12" t="s" s="17">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="AM12" t="s" s="18">
         <f>IF(A12="Top die - C4 bump",IF(AI12="inout","inout",IF(AI12="input","output",IF(AI12="output","input",""))),IF(A12="HBM - C4 bump",IF(AK12="inout","inout",IF(AK12="input","output",IF(AK12="output","input"))),""))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AN12" t="s" s="19">
         <f>AL12</f>
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="AO12" t="s" s="19">
         <f>IF(AM12="inout","inout",IF(AM12="input","output",IF(AM12="output","input","")))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AP12" t="s" s="19">
         <f>IF(AR12="Point-To-Point","HBM_"&amp;AU12&amp;"_DA"&amp;AS12,IF(AR12="Multi-Drop","HBM_"&amp;AT12&amp;"_DA"&amp;AS12,IF(AR12="High-Z","",IF(AN12="","",RIGHT(AN12,LEN(AN12)-3)))))</f>
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="AQ12" t="s" s="19">
         <f>IF(AO12="inout","inout",IF(AO12="input","output",IF(AO12="output","input","")))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AR12" s="20"/>
       <c r="AS12" s="19"/>
@@ -4375,11 +4402,11 @@
       </c>
       <c r="AY12" t="s" s="8">
         <f>IF(F12="","",IF(A12="Top die - HBM","SII_L_"&amp;F12,"L_"&amp;F12))</f>
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="AZ12" t="s" s="8">
         <f>_xlfn.FORMULATEXT(AY12)</f>
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="BA12" t="b" s="22">
         <f>EXACT(TRIM(_xlfn.FORMULATEXT(AP12)),TRIM(BC12))</f>
@@ -4387,36 +4414,36 @@
       </c>
       <c r="BB12" t="s" s="8">
         <f>IF(AN12="","","C_"&amp;RIGHT(AN12,LEN(AN12)-3))</f>
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="BC12" t="s" s="8">
         <f>_xlfn.FORMULATEXT(BB12)</f>
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="BD12" s="23"/>
       <c r="BE12" s="23"/>
     </row>
     <row r="13" ht="13.55" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s" s="8">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s" s="8">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D13" t="s" s="8">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="E13" t="s" s="8">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="F13" t="s" s="9">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="G13" t="s" s="10">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H13" t="s" s="10">
         <v>64</v>
@@ -4474,38 +4501,38 @@
       <c r="AG13" s="11"/>
       <c r="AH13" t="s" s="13">
         <f>IF(OR(F13="",LEFT(F13,3)="NC_"),"",IF(A13="Top die - HBM","SII_L_"&amp;F13,"L_"&amp;F13))</f>
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="AI13" t="s" s="14">
         <f>IF(LEFT(F13,3)="NC_","",IF(OR(A13="Top die - C4 bump",A13="Top die - HBM"),IF(G13="inout","inout",IF(G13="input","output",IF(G13="output","input"))),""))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AJ13" s="15"/>
       <c r="AK13" t="s" s="16">
         <f>IF(A13="HBM - C4 bump","inout",IF(A13="Top die - HBM",IF(AI13="inout","inout",IF(AI13="input","output",IF(AI13="output","input"))),""))</f>
       </c>
       <c r="AL13" t="s" s="17">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="AM13" t="s" s="18">
         <f>IF(A13="Top die - C4 bump",IF(AI13="inout","inout",IF(AI13="input","output",IF(AI13="output","input",""))),IF(A13="HBM - C4 bump",IF(AK13="inout","inout",IF(AK13="input","output",IF(AK13="output","input"))),""))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AN13" t="s" s="19">
         <f>AL13</f>
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="AO13" t="s" s="19">
         <f>IF(AM13="inout","inout",IF(AM13="input","output",IF(AM13="output","input","")))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AP13" t="s" s="19">
         <f>IF(AR13="Point-To-Point","HBM_"&amp;AU13&amp;"_DA"&amp;AS13,IF(AR13="Multi-Drop","HBM_"&amp;AT13&amp;"_DA"&amp;AS13,IF(AR13="High-Z","",IF(AN13="","",RIGHT(AN13,LEN(AN13)-3)))))</f>
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="AQ13" t="s" s="19">
         <f>IF(AO13="inout","inout",IF(AO13="input","output",IF(AO13="output","input","")))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AR13" s="20"/>
       <c r="AS13" s="19"/>
@@ -4524,11 +4551,11 @@
       </c>
       <c r="AY13" t="s" s="8">
         <f>IF(F13="","",IF(A13="Top die - HBM","SII_L_"&amp;F13,"L_"&amp;F13))</f>
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="AZ13" t="s" s="8">
         <f>_xlfn.FORMULATEXT(AY13)</f>
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="BA13" t="b" s="22">
         <f>EXACT(TRIM(_xlfn.FORMULATEXT(AP13)),TRIM(BC13))</f>
@@ -4536,36 +4563,36 @@
       </c>
       <c r="BB13" t="s" s="8">
         <f>IF(AN13="","","C_"&amp;RIGHT(AN13,LEN(AN13)-3))</f>
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="BC13" t="s" s="8">
         <f>_xlfn.FORMULATEXT(BB13)</f>
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="BD13" s="23"/>
       <c r="BE13" s="23"/>
     </row>
     <row r="14" ht="13.55" customHeight="1">
       <c r="A14" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B14" t="s" s="8">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C14" t="s" s="8">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D14" t="s" s="8">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E14" t="s" s="8">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="F14" t="s" s="9">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="G14" t="s" s="10">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H14" t="s" s="10">
         <v>64</v>
@@ -4595,7 +4622,7 @@
         <v>65</v>
       </c>
       <c r="U14" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="V14" s="12">
         <v>0</v>
@@ -4621,42 +4648,42 @@
         <v>65</v>
       </c>
       <c r="AG14" t="s" s="10">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="AH14" t="s" s="13">
         <f>IF(OR(F14="",LEFT(F14,3)="NC_"),"",IF(A14="Top die - HBM","SII_L_"&amp;F14,"L_"&amp;F14))</f>
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="AI14" t="s" s="14">
         <f>IF(LEFT(F14,3)="NC_","",IF(OR(A14="Top die - C4 bump",A14="Top die - HBM"),IF(G14="inout","inout",IF(G14="input","output",IF(G14="output","input"))),""))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AJ14" s="15"/>
       <c r="AK14" t="s" s="16">
         <f>IF(A14="HBM - C4 bump","inout",IF(A14="Top die - HBM",IF(AI14="inout","inout",IF(AI14="input","output",IF(AI14="output","input"))),""))</f>
       </c>
       <c r="AL14" t="s" s="17">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="AM14" t="s" s="18">
         <f>IF(A14="Top die - C4 bump",IF(AI14="inout","inout",IF(AI14="input","output",IF(AI14="output","input",""))),IF(A14="HBM - C4 bump",IF(AK14="inout","inout",IF(AK14="input","output",IF(AK14="output","input"))),""))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AN14" t="s" s="19">
         <f>AL14</f>
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="AO14" t="s" s="19">
         <f>IF(AM14="inout","inout",IF(AM14="input","output",IF(AM14="output","input","")))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AP14" t="s" s="19">
         <f>IF(AR14="Point-To-Point","HBM_"&amp;AU14&amp;"_DA"&amp;AS14,IF(AR14="Multi-Drop","HBM_"&amp;AT14&amp;"_DA"&amp;AS14,IF(AR14="High-Z","",IF(AN14="","",RIGHT(AN14,LEN(AN14)-3)))))</f>
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="AQ14" t="s" s="19">
         <f>IF(AO14="inout","inout",IF(AO14="input","output",IF(AO14="output","input","")))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AR14" s="20"/>
       <c r="AS14" s="19"/>
@@ -4675,11 +4702,11 @@
       </c>
       <c r="AY14" t="s" s="8">
         <f>IF(F14="","",IF(A14="Top die - HBM","SII_L_"&amp;F14,"L_"&amp;F14))</f>
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="AZ14" t="s" s="8">
         <f>_xlfn.FORMULATEXT(AY14)</f>
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="BA14" t="b" s="22">
         <f>EXACT(TRIM(_xlfn.FORMULATEXT(AP14)),TRIM(BC14))</f>
@@ -4687,36 +4714,36 @@
       </c>
       <c r="BB14" t="s" s="8">
         <f>IF(AN14="","","C_"&amp;RIGHT(AN14,LEN(AN14)-3))</f>
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="BC14" t="s" s="8">
         <f>_xlfn.FORMULATEXT(BB14)</f>
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="BD14" s="23"/>
       <c r="BE14" s="23"/>
     </row>
     <row r="15" ht="13.55" customHeight="1">
       <c r="A15" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s" s="8">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s" s="8">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D15" t="s" s="8">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E15" t="s" s="8">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="F15" t="s" s="9">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="G15" t="s" s="10">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H15" t="s" s="10">
         <v>64</v>
@@ -4746,7 +4773,7 @@
         <v>65</v>
       </c>
       <c r="U15" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="V15" s="12">
         <v>0</v>
@@ -4772,42 +4799,42 @@
         <v>65</v>
       </c>
       <c r="AG15" t="s" s="10">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="AH15" t="s" s="13">
         <f>IF(OR(F15="",LEFT(F15,3)="NC_"),"",IF(A15="Top die - HBM","SII_L_"&amp;F15,"L_"&amp;F15))</f>
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="AI15" t="s" s="14">
         <f>IF(LEFT(F15,3)="NC_","",IF(OR(A15="Top die - C4 bump",A15="Top die - HBM"),IF(G15="inout","inout",IF(G15="input","output",IF(G15="output","input"))),""))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AJ15" s="15"/>
       <c r="AK15" t="s" s="16">
         <f>IF(A15="HBM - C4 bump","inout",IF(A15="Top die - HBM",IF(AI15="inout","inout",IF(AI15="input","output",IF(AI15="output","input"))),""))</f>
       </c>
       <c r="AL15" t="s" s="17">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="AM15" t="s" s="18">
         <f>IF(A15="Top die - C4 bump",IF(AI15="inout","inout",IF(AI15="input","output",IF(AI15="output","input",""))),IF(A15="HBM - C4 bump",IF(AK15="inout","inout",IF(AK15="input","output",IF(AK15="output","input"))),""))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AN15" t="s" s="19">
         <f>AL15</f>
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="AO15" t="s" s="19">
         <f>IF(AM15="inout","inout",IF(AM15="input","output",IF(AM15="output","input","")))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AP15" t="s" s="19">
         <f>IF(AR15="Point-To-Point","HBM_"&amp;AU15&amp;"_DA"&amp;AS15,IF(AR15="Multi-Drop","HBM_"&amp;AT15&amp;"_DA"&amp;AS15,IF(AR15="High-Z","",IF(AN15="","",RIGHT(AN15,LEN(AN15)-3)))))</f>
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="AQ15" t="s" s="19">
         <f>IF(AO15="inout","inout",IF(AO15="input","output",IF(AO15="output","input","")))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AR15" s="20"/>
       <c r="AS15" s="19"/>
@@ -4826,11 +4853,11 @@
       </c>
       <c r="AY15" t="s" s="8">
         <f>IF(F15="","",IF(A15="Top die - HBM","SII_L_"&amp;F15,"L_"&amp;F15))</f>
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="AZ15" t="s" s="8">
         <f>_xlfn.FORMULATEXT(AY15)</f>
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="BA15" t="b" s="22">
         <f>EXACT(TRIM(_xlfn.FORMULATEXT(AP15)),TRIM(BC15))</f>
@@ -4838,36 +4865,36 @@
       </c>
       <c r="BB15" t="s" s="8">
         <f>IF(AN15="","","C_"&amp;RIGHT(AN15,LEN(AN15)-3))</f>
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="BC15" t="s" s="8">
         <f>_xlfn.FORMULATEXT(BB15)</f>
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="BD15" s="23"/>
       <c r="BE15" s="23"/>
     </row>
     <row r="16" ht="13.55" customHeight="1">
       <c r="A16" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s" s="8">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C16" t="s" s="8">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D16" t="s" s="8">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E16" t="s" s="8">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F16" t="s" s="9">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="G16" t="s" s="10">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H16" t="s" s="10">
         <v>64</v>
@@ -4897,7 +4924,7 @@
         <v>65</v>
       </c>
       <c r="U16" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="V16" s="12">
         <v>0</v>
@@ -4923,42 +4950,42 @@
         <v>65</v>
       </c>
       <c r="AG16" t="s" s="10">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="AH16" t="s" s="13">
         <f>IF(OR(F16="",LEFT(F16,3)="NC_"),"",IF(A16="Top die - HBM","SII_L_"&amp;F16,"L_"&amp;F16))</f>
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="AI16" t="s" s="14">
         <f>IF(LEFT(F16,3)="NC_","",IF(OR(A16="Top die - C4 bump",A16="Top die - HBM"),IF(G16="inout","inout",IF(G16="input","output",IF(G16="output","input"))),""))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AJ16" s="15"/>
       <c r="AK16" t="s" s="16">
         <f>IF(A16="HBM - C4 bump","inout",IF(A16="Top die - HBM",IF(AI16="inout","inout",IF(AI16="input","output",IF(AI16="output","input"))),""))</f>
       </c>
       <c r="AL16" t="s" s="17">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="AM16" t="s" s="18">
         <f>IF(A16="Top die - C4 bump",IF(AI16="inout","inout",IF(AI16="input","output",IF(AI16="output","input",""))),IF(A16="HBM - C4 bump",IF(AK16="inout","inout",IF(AK16="input","output",IF(AK16="output","input"))),""))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AN16" t="s" s="19">
         <f>AL16</f>
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="AO16" t="s" s="19">
         <f>IF(AM16="inout","inout",IF(AM16="input","output",IF(AM16="output","input","")))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AP16" t="s" s="19">
         <f>IF(AR16="Point-To-Point","HBM_"&amp;AU16&amp;"_DA"&amp;AS16,IF(AR16="Multi-Drop","HBM_"&amp;AT16&amp;"_DA"&amp;AS16,IF(AR16="High-Z","",IF(AN16="","",RIGHT(AN16,LEN(AN16)-3)))))</f>
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="AQ16" t="s" s="19">
         <f>IF(AO16="inout","inout",IF(AO16="input","output",IF(AO16="output","input","")))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AR16" s="20"/>
       <c r="AS16" s="19"/>
@@ -4977,11 +5004,11 @@
       </c>
       <c r="AY16" t="s" s="8">
         <f>IF(F16="","",IF(A16="Top die - HBM","SII_L_"&amp;F16,"L_"&amp;F16))</f>
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="AZ16" t="s" s="8">
         <f>_xlfn.FORMULATEXT(AY16)</f>
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="BA16" t="b" s="22">
         <f>EXACT(TRIM(_xlfn.FORMULATEXT(AP16)),TRIM(BC16))</f>
@@ -4989,36 +5016,36 @@
       </c>
       <c r="BB16" t="s" s="8">
         <f>IF(AN16="","","C_"&amp;RIGHT(AN16,LEN(AN16)-3))</f>
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="BC16" t="s" s="8">
         <f>_xlfn.FORMULATEXT(BB16)</f>
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="BD16" s="23"/>
       <c r="BE16" s="23"/>
     </row>
     <row r="17" ht="13.55" customHeight="1">
       <c r="A17" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s" s="8">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s" s="8">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D17" t="s" s="8">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E17" t="s" s="8">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F17" t="s" s="9">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="G17" t="s" s="10">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H17" t="s" s="10">
         <v>64</v>
@@ -5048,7 +5075,7 @@
         <v>65</v>
       </c>
       <c r="U17" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="V17" s="12">
         <v>0</v>
@@ -5074,42 +5101,42 @@
         <v>65</v>
       </c>
       <c r="AG17" t="s" s="10">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="AH17" t="s" s="13">
         <f>IF(OR(F17="",LEFT(F17,3)="NC_"),"",IF(A17="Top die - HBM","SII_L_"&amp;F17,"L_"&amp;F17))</f>
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="AI17" t="s" s="14">
         <f>IF(LEFT(F17,3)="NC_","",IF(OR(A17="Top die - C4 bump",A17="Top die - HBM"),IF(G17="inout","inout",IF(G17="input","output",IF(G17="output","input"))),""))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AJ17" s="15"/>
       <c r="AK17" t="s" s="16">
         <f>IF(A17="HBM - C4 bump","inout",IF(A17="Top die - HBM",IF(AI17="inout","inout",IF(AI17="input","output",IF(AI17="output","input"))),""))</f>
       </c>
       <c r="AL17" t="s" s="17">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="AM17" t="s" s="18">
         <f>IF(A17="Top die - C4 bump",IF(AI17="inout","inout",IF(AI17="input","output",IF(AI17="output","input",""))),IF(A17="HBM - C4 bump",IF(AK17="inout","inout",IF(AK17="input","output",IF(AK17="output","input"))),""))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AN17" t="s" s="19">
         <f>AL17</f>
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="AO17" t="s" s="19">
         <f>IF(AM17="inout","inout",IF(AM17="input","output",IF(AM17="output","input","")))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AP17" t="s" s="19">
         <f>IF(AR17="Point-To-Point","HBM_"&amp;AU17&amp;"_DA"&amp;AS17,IF(AR17="Multi-Drop","HBM_"&amp;AT17&amp;"_DA"&amp;AS17,IF(AR17="High-Z","",IF(AN17="","",RIGHT(AN17,LEN(AN17)-3)))))</f>
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="AQ17" t="s" s="19">
         <f>IF(AO17="inout","inout",IF(AO17="input","output",IF(AO17="output","input","")))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AR17" s="20"/>
       <c r="AS17" s="19"/>
@@ -5128,11 +5155,11 @@
       </c>
       <c r="AY17" t="s" s="8">
         <f>IF(F17="","",IF(A17="Top die - HBM","SII_L_"&amp;F17,"L_"&amp;F17))</f>
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="AZ17" t="s" s="8">
         <f>_xlfn.FORMULATEXT(AY17)</f>
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="BA17" t="b" s="22">
         <f>EXACT(TRIM(_xlfn.FORMULATEXT(AP17)),TRIM(BC17))</f>
@@ -5140,36 +5167,36 @@
       </c>
       <c r="BB17" t="s" s="8">
         <f>IF(AN17="","","C_"&amp;RIGHT(AN17,LEN(AN17)-3))</f>
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="BC17" t="s" s="8">
         <f>_xlfn.FORMULATEXT(BB17)</f>
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="BD17" s="23"/>
       <c r="BE17" s="23"/>
     </row>
     <row r="18" ht="13.55" customHeight="1">
       <c r="A18" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B18" t="s" s="8">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C18" t="s" s="8">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D18" t="s" s="8">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E18" t="s" s="8">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="F18" t="s" s="9">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="G18" t="s" s="10">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="H18" t="s" s="10">
         <v>64</v>
@@ -5215,54 +5242,54 @@
         <v>65</v>
       </c>
       <c r="AC18" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="AD18" s="12">
         <v>0</v>
       </c>
       <c r="AE18" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="AF18" s="12">
         <v>0</v>
       </c>
       <c r="AG18" t="s" s="10">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="AH18" t="s" s="13">
         <f>IF(OR(F18="",LEFT(F18,3)="NC_"),"",IF(A18="Top die - HBM","SII_L_"&amp;F18,"L_"&amp;F18))</f>
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="AI18" t="s" s="14">
         <f>IF(LEFT(F18,3)="NC_","",IF(OR(A18="Top die - C4 bump",A18="Top die - HBM"),IF(G18="inout","inout",IF(G18="input","output",IF(G18="output","input"))),""))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AJ18" s="15"/>
       <c r="AK18" t="s" s="16">
         <f>IF(A18="HBM - C4 bump","inout",IF(A18="Top die - HBM",IF(AI18="inout","inout",IF(AI18="input","output",IF(AI18="output","input"))),""))</f>
       </c>
       <c r="AL18" t="s" s="17">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="AM18" t="s" s="18">
         <f>IF(A18="Top die - C4 bump",IF(AI18="inout","inout",IF(AI18="input","output",IF(AI18="output","input",""))),IF(A18="HBM - C4 bump",IF(AK18="inout","inout",IF(AK18="input","output",IF(AK18="output","input"))),""))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AN18" t="s" s="19">
         <f>AL18</f>
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="AO18" t="s" s="19">
         <f>IF(AM18="inout","inout",IF(AM18="input","output",IF(AM18="output","input","")))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AP18" t="s" s="19">
         <f>IF(AR18="Point-To-Point","HBM_"&amp;AU18&amp;"_DA"&amp;AS18,IF(AR18="Multi-Drop","HBM_"&amp;AT18&amp;"_DA"&amp;AS18,IF(AR18="High-Z","",IF(AN18="","",RIGHT(AN18,LEN(AN18)-3)))))</f>
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="AQ18" t="s" s="19">
         <f>IF(AO18="inout","inout",IF(AO18="input","output",IF(AO18="output","input","")))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AR18" s="20"/>
       <c r="AS18" s="19"/>
@@ -5283,25 +5310,25 @@
     </row>
     <row r="19" ht="13.55" customHeight="1">
       <c r="A19" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B19" t="s" s="8">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C19" t="s" s="8">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D19" t="s" s="8">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E19" t="s" s="8">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="F19" t="s" s="9">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="G19" t="s" s="10">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="H19" t="s" s="10">
         <v>64</v>
@@ -5347,54 +5374,54 @@
         <v>65</v>
       </c>
       <c r="AC19" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="AD19" s="12">
         <v>0</v>
       </c>
       <c r="AE19" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="AF19" s="12">
         <v>0</v>
       </c>
       <c r="AG19" t="s" s="10">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="AH19" t="s" s="13">
         <f>IF(OR(F19="",LEFT(F19,3)="NC_"),"",IF(A19="Top die - HBM","SII_L_"&amp;F19,"L_"&amp;F19))</f>
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="AI19" t="s" s="14">
         <f>IF(LEFT(F19,3)="NC_","",IF(OR(A19="Top die - C4 bump",A19="Top die - HBM"),IF(G19="inout","inout",IF(G19="input","output",IF(G19="output","input"))),""))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AJ19" s="15"/>
       <c r="AK19" t="s" s="16">
         <f>IF(A19="HBM - C4 bump","inout",IF(A19="Top die - HBM",IF(AI19="inout","inout",IF(AI19="input","output",IF(AI19="output","input"))),""))</f>
       </c>
       <c r="AL19" t="s" s="17">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="AM19" t="s" s="18">
         <f>IF(A19="Top die - C4 bump",IF(AI19="inout","inout",IF(AI19="input","output",IF(AI19="output","input",""))),IF(A19="HBM - C4 bump",IF(AK19="inout","inout",IF(AK19="input","output",IF(AK19="output","input"))),""))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AN19" t="s" s="19">
         <f>AL19</f>
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="AO19" t="s" s="19">
         <f>IF(AM19="inout","inout",IF(AM19="input","output",IF(AM19="output","input","")))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AP19" t="s" s="19">
         <f>IF(AR19="Point-To-Point","HBM_"&amp;AU19&amp;"_DA"&amp;AS19,IF(AR19="Multi-Drop","HBM_"&amp;AT19&amp;"_DA"&amp;AS19,IF(AR19="High-Z","",IF(AN19="","",RIGHT(AN19,LEN(AN19)-3)))))</f>
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="AQ19" t="s" s="19">
         <f>IF(AO19="inout","inout",IF(AO19="input","output",IF(AO19="output","input","")))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AR19" s="20"/>
       <c r="AS19" s="19"/>
@@ -5415,25 +5442,25 @@
     </row>
     <row r="20" ht="13.55" customHeight="1">
       <c r="A20" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B20" t="s" s="8">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C20" t="s" s="8">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D20" t="s" s="8">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E20" t="s" s="8">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F20" t="s" s="9">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="G20" t="s" s="10">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="H20" t="s" s="10">
         <v>64</v>
@@ -5479,54 +5506,54 @@
         <v>65</v>
       </c>
       <c r="AC20" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="AD20" s="12">
         <v>0</v>
       </c>
       <c r="AE20" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="AF20" s="12">
         <v>0</v>
       </c>
       <c r="AG20" t="s" s="10">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="AH20" t="s" s="13">
         <f>IF(OR(F20="",LEFT(F20,3)="NC_"),"",IF(A20="Top die - HBM","SII_L_"&amp;F20,"L_"&amp;F20))</f>
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="AI20" t="s" s="14">
         <f>IF(LEFT(F20,3)="NC_","",IF(OR(A20="Top die - C4 bump",A20="Top die - HBM"),IF(G20="inout","inout",IF(G20="input","output",IF(G20="output","input"))),""))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AJ20" s="15"/>
       <c r="AK20" t="s" s="16">
         <f>IF(A20="HBM - C4 bump","inout",IF(A20="Top die - HBM",IF(AI20="inout","inout",IF(AI20="input","output",IF(AI20="output","input"))),""))</f>
       </c>
       <c r="AL20" t="s" s="17">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="AM20" t="s" s="18">
         <f>IF(A20="Top die - C4 bump",IF(AI20="inout","inout",IF(AI20="input","output",IF(AI20="output","input",""))),IF(A20="HBM - C4 bump",IF(AK20="inout","inout",IF(AK20="input","output",IF(AK20="output","input"))),""))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AN20" t="s" s="19">
         <f>AL20</f>
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="AO20" t="s" s="19">
         <f>IF(AM20="inout","inout",IF(AM20="input","output",IF(AM20="output","input","")))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AP20" t="s" s="19">
         <f>IF(AR20="Point-To-Point","HBM_"&amp;AU20&amp;"_DA"&amp;AS20,IF(AR20="Multi-Drop","HBM_"&amp;AT20&amp;"_DA"&amp;AS20,IF(AR20="High-Z","",IF(AN20="","",RIGHT(AN20,LEN(AN20)-3)))))</f>
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="AQ20" t="s" s="19">
         <f>IF(AO20="inout","inout",IF(AO20="input","output",IF(AO20="output","input","")))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AR20" s="20"/>
       <c r="AS20" s="19"/>
@@ -5547,25 +5574,25 @@
     </row>
     <row r="21" ht="13.55" customHeight="1">
       <c r="A21" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B21" t="s" s="8">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C21" t="s" s="8">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D21" t="s" s="8">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E21" t="s" s="8">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F21" t="s" s="9">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="G21" t="s" s="10">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="H21" t="s" s="10">
         <v>64</v>
@@ -5611,54 +5638,54 @@
         <v>65</v>
       </c>
       <c r="AC21" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="AD21" s="12">
         <v>0</v>
       </c>
       <c r="AE21" t="s" s="10">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="AF21" s="12">
         <v>0</v>
       </c>
       <c r="AG21" t="s" s="10">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="AH21" t="s" s="13">
         <f>IF(OR(F21="",LEFT(F21,3)="NC_"),"",IF(A21="Top die - HBM","SII_L_"&amp;F21,"L_"&amp;F21))</f>
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="AI21" t="s" s="14">
         <f>IF(LEFT(F21,3)="NC_","",IF(OR(A21="Top die - C4 bump",A21="Top die - HBM"),IF(G21="inout","inout",IF(G21="input","output",IF(G21="output","input"))),""))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AJ21" s="15"/>
       <c r="AK21" t="s" s="16">
         <f>IF(A21="HBM - C4 bump","inout",IF(A21="Top die - HBM",IF(AI21="inout","inout",IF(AI21="input","output",IF(AI21="output","input"))),""))</f>
       </c>
       <c r="AL21" t="s" s="17">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="AM21" t="s" s="18">
         <f>IF(A21="Top die - C4 bump",IF(AI21="inout","inout",IF(AI21="input","output",IF(AI21="output","input",""))),IF(A21="HBM - C4 bump",IF(AK21="inout","inout",IF(AK21="input","output",IF(AK21="output","input"))),""))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AN21" t="s" s="19">
         <f>AL21</f>
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="AO21" t="s" s="19">
         <f>IF(AM21="inout","inout",IF(AM21="input","output",IF(AM21="output","input","")))</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AP21" t="s" s="19">
         <f>IF(AR21="Point-To-Point","HBM_"&amp;AU21&amp;"_DA"&amp;AS21,IF(AR21="Multi-Drop","HBM_"&amp;AT21&amp;"_DA"&amp;AS21,IF(AR21="High-Z","",IF(AN21="","",RIGHT(AN21,LEN(AN21)-3)))))</f>
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="AQ21" t="s" s="19">
         <f>IF(AO21="inout","inout",IF(AO21="input","output",IF(AO21="output","input","")))</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AR21" s="20"/>
       <c r="AS21" s="19"/>
@@ -5679,26 +5706,26 @@
     </row>
     <row r="22" ht="13.55" customHeight="1">
       <c r="A22" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B22" t="s" s="8">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C22" t="s" s="8">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D22" t="s" s="8">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="E22" s="21"/>
       <c r="F22" t="s" s="9">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="G22" t="s" s="10">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H22" t="s" s="10">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
@@ -5770,26 +5797,26 @@
     </row>
     <row r="23" ht="13.55" customHeight="1">
       <c r="A23" t="s" s="7">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="B23" t="s" s="8">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C23" t="s" s="8">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D23" t="s" s="8">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" t="s" s="9">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="G23" t="s" s="10">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H23" t="s" s="10">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>

</xml_diff>